<commit_message>
Add Jenkinsfile for Playwright CI
</commit_message>
<xml_diff>
--- a/tests/DATA/ACSTD AllState.xlsx
+++ b/tests/DATA/ACSTD AllState.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avelm\Desktop\RESTD Jenkins\tests\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C31A64-1E4F-4C83-8C20-6C9AB5B177E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2C731A-C35A-49F6-9959-864E19B6FCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,7 +937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -981,86 +981,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1346,10 +1267,16 @@
   <dimension ref="A1:AM42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AM42"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
@@ -4725,200 +4652,200 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:39">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="30" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="31" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="31" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="31" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="31" t="s">
+      <c r="AA1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="31" t="s">
+      <c r="AB1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="31" t="s">
+      <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="32" t="s">
+      <c r="AD1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="33" t="s">
+      <c r="AE1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="33" t="s">
+      <c r="AF1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="34" t="s">
+      <c r="AG1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="34" t="s">
+      <c r="AH1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="34" t="s">
+      <c r="AI1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="34" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="34" t="s">
+      <c r="AK1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="34" t="s">
+      <c r="AL1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="35" t="s">
+      <c r="AM1" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:39">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="11">
         <v>46027</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="38" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="34" t="s">
+      <c r="J2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="40" t="s">
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="50" t="s">
+      <c r="X2" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="42" t="s">
+      <c r="Y2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="43" t="s">
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AG2" s="45" t="s">
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="AH2" s="46" t="s">
+      <c r="AH2" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="AI2" s="45" t="s">
+      <c r="AI2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AJ2" s="45" t="s">
+      <c r="AJ2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AK2" s="45"/>
-      <c r="AL2" s="45"/>
-      <c r="AM2" s="47" t="s">
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="20" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4938,516 +4865,516 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:39">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="51" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="51" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="54" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="54" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="54" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="54" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="54" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="54" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="55" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="55" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="55" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="55" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="55" t="s">
+      <c r="AA1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="55" t="s">
+      <c r="AB1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="55" t="s">
+      <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="56" t="s">
+      <c r="AD1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="57" t="s">
+      <c r="AE1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="57" t="s">
+      <c r="AF1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="58" t="s">
+      <c r="AG1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="58" t="s">
+      <c r="AH1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="58" t="s">
+      <c r="AI1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="58" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="58" t="s">
+      <c r="AK1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="58" t="s">
+      <c r="AL1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="59" t="s">
+      <c r="AM1" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:39">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="F2" s="61">
+      <c r="F2" s="11">
         <v>46040</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="62" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="76" t="s">
+      <c r="J2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="64" t="s">
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="74" t="s">
+      <c r="X2" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="Y2" s="66" t="s">
+      <c r="Y2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="67" t="s">
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AE2" s="68"/>
-      <c r="AF2" s="68"/>
-      <c r="AG2" s="69" t="s">
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="AH2" s="70" t="s">
+      <c r="AH2" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="AI2" s="69" t="s">
+      <c r="AI2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AJ2" s="69" t="s">
+      <c r="AJ2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AK2" s="69"/>
-      <c r="AL2" s="69"/>
-      <c r="AM2" s="71" t="s">
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:39">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="29" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="F3" s="61">
+      <c r="F3" s="11">
         <v>46040</v>
       </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="62" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="76" t="s">
+      <c r="J3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="72"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="64" t="s">
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="X3" s="74" t="s">
+      <c r="X3" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="Y3" s="66" t="s">
+      <c r="Y3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="66"/>
-      <c r="AB3" s="66"/>
-      <c r="AC3" s="66"/>
-      <c r="AD3" s="67" t="s">
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AE3" s="73"/>
-      <c r="AF3" s="73"/>
-      <c r="AG3" s="69" t="s">
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="23"/>
+      <c r="AG3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="AH3" s="70" t="s">
+      <c r="AH3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="AI3" s="69" t="s">
+      <c r="AI3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AJ3" s="69" t="s">
+      <c r="AJ3" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AK3" s="69"/>
-      <c r="AL3" s="69"/>
-      <c r="AM3" s="71" t="s">
+      <c r="AK3" s="18"/>
+      <c r="AL3" s="18"/>
+      <c r="AM3" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:39">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="F4" s="61">
+      <c r="F4" s="11">
         <v>46040</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="62" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="76" t="s">
+      <c r="J4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="64" t="s">
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="X4" s="74" t="s">
+      <c r="X4" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="Y4" s="66" t="s">
+      <c r="Y4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Z4" s="66"/>
-      <c r="AA4" s="66"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="67" t="s">
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="69" t="s">
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="AH4" s="70" t="s">
+      <c r="AH4" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="AI4" s="69" t="s">
+      <c r="AI4" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="AJ4" s="69" t="s">
+      <c r="AJ4" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AK4" s="69"/>
-      <c r="AL4" s="69"/>
-      <c r="AM4" s="71" t="s">
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:39">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="F5" s="61">
+      <c r="F5" s="11">
         <v>46031</v>
       </c>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="62" t="s">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60" t="s">
+      <c r="J5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="58"/>
-      <c r="U5" s="58"/>
-      <c r="V5" s="58"/>
-      <c r="W5" s="64" t="s">
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="X5" s="74" t="s">
+      <c r="X5" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="Y5" s="66" t="s">
+      <c r="Y5" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Z5" s="66"/>
-      <c r="AA5" s="66"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
-      <c r="AD5" s="67" t="s">
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AE5" s="73"/>
-      <c r="AF5" s="73"/>
-      <c r="AG5" s="69" t="s">
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="AH5" s="70" t="s">
+      <c r="AH5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="AI5" s="69" t="s">
+      <c r="AI5" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AJ5" s="69" t="s">
+      <c r="AJ5" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AK5" s="69"/>
-      <c r="AL5" s="69"/>
-      <c r="AM5" s="71" t="s">
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="18"/>
+      <c r="AM5" s="20" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:39">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="F6" s="61">
+      <c r="F6" s="11">
         <v>46040</v>
       </c>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="62" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60" t="s">
+      <c r="J6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="64" t="s">
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="X6" s="74" t="s">
+      <c r="X6" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="Y6" s="66" t="s">
+      <c r="Y6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Z6" s="66"/>
-      <c r="AA6" s="66"/>
-      <c r="AB6" s="66"/>
-      <c r="AC6" s="66"/>
-      <c r="AD6" s="67" t="s">
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AE6" s="73"/>
-      <c r="AF6" s="73"/>
-      <c r="AG6" s="69" t="s">
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="AH6" s="70" t="s">
+      <c r="AH6" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="AI6" s="69" t="s">
+      <c r="AI6" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AJ6" s="69" t="s">
+      <c r="AJ6" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AK6" s="69"/>
-      <c r="AL6" s="69"/>
-      <c r="AM6" s="71" t="s">
+      <c r="AK6" s="18"/>
+      <c r="AL6" s="18"/>
+      <c r="AM6" s="20" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>